<commit_message>
version2.0 of Gnatt chart
</commit_message>
<xml_diff>
--- a/CS401ProjectGnattChart.xlsx
+++ b/CS401ProjectGnattChart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="147" documentId="13_ncr:1_{93D8DC03-8DEF-45F2-8570-FF4EF3D5A7AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0C671F95-1333-4A98-97AA-F09DDF8D8779}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="13_ncr:1_{93D8DC03-8DEF-45F2-8570-FF4EF3D5A7AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{30FDB64F-CD98-4F5D-8587-BFAFE0986624}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -279,15 +279,6 @@
     <t>Debug</t>
   </si>
   <si>
-    <t>Model Analysis</t>
-  </si>
-  <si>
-    <t>Analysis Diagram</t>
-  </si>
-  <si>
-    <t>Model Interaction</t>
-  </si>
-  <si>
     <t>Implementt GUI Emergency buttons</t>
   </si>
   <si>
@@ -310,6 +301,15 @@
   </si>
   <si>
     <t>Implement Client/Newsfeed/password to Monitor</t>
+  </si>
+  <si>
+    <t>Design specification</t>
+  </si>
+  <si>
+    <t>OO(object-oriented) Analysis</t>
+  </si>
+  <si>
+    <t>Model Interaction [Use Cases/Test Plan]</t>
   </si>
 </sst>
 </file>
@@ -919,6 +919,21 @@
     <xf numFmtId="9" fontId="22" fillId="6" borderId="11" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="8" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -926,21 +941,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="8" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="3" builtinId="3" customBuiltin="1"/>
@@ -1810,8 +1810,8 @@
   <dimension ref="A1:BS49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="83" zoomScaleNormal="40" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5:G5"/>
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1859,127 +1859,127 @@
         <v>25</v>
       </c>
       <c r="B3" s="34"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="74">
+      <c r="D3" s="74"/>
+      <c r="E3" s="72">
         <v>43878</v>
       </c>
-      <c r="F3" s="74"/>
+      <c r="F3" s="72"/>
     </row>
     <row r="4" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="68" t="s">
+      <c r="C4" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="69"/>
+      <c r="D4" s="74"/>
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="71">
+      <c r="I4" s="69">
         <f>I5</f>
         <v>43878</v>
       </c>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="72"/>
-      <c r="N4" s="72"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="71">
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="70"/>
+      <c r="O4" s="71"/>
+      <c r="P4" s="69">
         <f>P5</f>
         <v>43885</v>
       </c>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="72"/>
-      <c r="S4" s="72"/>
-      <c r="T4" s="72"/>
-      <c r="U4" s="72"/>
-      <c r="V4" s="73"/>
-      <c r="W4" s="71">
+      <c r="Q4" s="70"/>
+      <c r="R4" s="70"/>
+      <c r="S4" s="70"/>
+      <c r="T4" s="70"/>
+      <c r="U4" s="70"/>
+      <c r="V4" s="71"/>
+      <c r="W4" s="69">
         <f>W5</f>
         <v>43892</v>
       </c>
-      <c r="X4" s="72"/>
-      <c r="Y4" s="72"/>
-      <c r="Z4" s="72"/>
-      <c r="AA4" s="72"/>
-      <c r="AB4" s="72"/>
-      <c r="AC4" s="73"/>
-      <c r="AD4" s="71">
+      <c r="X4" s="70"/>
+      <c r="Y4" s="70"/>
+      <c r="Z4" s="70"/>
+      <c r="AA4" s="70"/>
+      <c r="AB4" s="70"/>
+      <c r="AC4" s="71"/>
+      <c r="AD4" s="69">
         <f>AD5</f>
         <v>43899</v>
       </c>
-      <c r="AE4" s="72"/>
-      <c r="AF4" s="72"/>
-      <c r="AG4" s="72"/>
-      <c r="AH4" s="72"/>
-      <c r="AI4" s="72"/>
-      <c r="AJ4" s="73"/>
-      <c r="AK4" s="71">
+      <c r="AE4" s="70"/>
+      <c r="AF4" s="70"/>
+      <c r="AG4" s="70"/>
+      <c r="AH4" s="70"/>
+      <c r="AI4" s="70"/>
+      <c r="AJ4" s="71"/>
+      <c r="AK4" s="69">
         <f>AK5</f>
         <v>43906</v>
       </c>
-      <c r="AL4" s="72"/>
-      <c r="AM4" s="72"/>
-      <c r="AN4" s="72"/>
-      <c r="AO4" s="72"/>
-      <c r="AP4" s="72"/>
-      <c r="AQ4" s="73"/>
-      <c r="AR4" s="71">
+      <c r="AL4" s="70"/>
+      <c r="AM4" s="70"/>
+      <c r="AN4" s="70"/>
+      <c r="AO4" s="70"/>
+      <c r="AP4" s="70"/>
+      <c r="AQ4" s="71"/>
+      <c r="AR4" s="69">
         <f>AR5</f>
         <v>43913</v>
       </c>
-      <c r="AS4" s="72"/>
-      <c r="AT4" s="72"/>
-      <c r="AU4" s="72"/>
-      <c r="AV4" s="72"/>
-      <c r="AW4" s="72"/>
-      <c r="AX4" s="73"/>
-      <c r="AY4" s="71">
+      <c r="AS4" s="70"/>
+      <c r="AT4" s="70"/>
+      <c r="AU4" s="70"/>
+      <c r="AV4" s="70"/>
+      <c r="AW4" s="70"/>
+      <c r="AX4" s="71"/>
+      <c r="AY4" s="69">
         <f>AY5</f>
         <v>43920</v>
       </c>
-      <c r="AZ4" s="72"/>
-      <c r="BA4" s="72"/>
-      <c r="BB4" s="72"/>
-      <c r="BC4" s="72"/>
-      <c r="BD4" s="72"/>
-      <c r="BE4" s="73"/>
-      <c r="BF4" s="71">
+      <c r="AZ4" s="70"/>
+      <c r="BA4" s="70"/>
+      <c r="BB4" s="70"/>
+      <c r="BC4" s="70"/>
+      <c r="BD4" s="70"/>
+      <c r="BE4" s="71"/>
+      <c r="BF4" s="69">
         <f>BF5</f>
         <v>43927</v>
       </c>
-      <c r="BG4" s="72"/>
-      <c r="BH4" s="72"/>
-      <c r="BI4" s="72"/>
-      <c r="BJ4" s="72"/>
-      <c r="BK4" s="72"/>
-      <c r="BL4" s="73"/>
-      <c r="BM4" s="71">
+      <c r="BG4" s="70"/>
+      <c r="BH4" s="70"/>
+      <c r="BI4" s="70"/>
+      <c r="BJ4" s="70"/>
+      <c r="BK4" s="70"/>
+      <c r="BL4" s="71"/>
+      <c r="BM4" s="69">
         <f>BM5</f>
         <v>43934</v>
       </c>
-      <c r="BN4" s="72"/>
-      <c r="BO4" s="72"/>
-      <c r="BP4" s="72"/>
-      <c r="BQ4" s="72"/>
-      <c r="BR4" s="72"/>
-      <c r="BS4" s="73"/>
+      <c r="BN4" s="70"/>
+      <c r="BO4" s="70"/>
+      <c r="BP4" s="70"/>
+      <c r="BQ4" s="70"/>
+      <c r="BR4" s="70"/>
+      <c r="BS4" s="71"/>
     </row>
     <row r="5" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
       <c r="I5" s="10">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43878</v>
@@ -3005,11 +3005,11 @@
     <row r="13" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="28"/>
       <c r="B13" s="39" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C13" s="40"/>
       <c r="D13" s="41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="42">
         <v>43885</v>
@@ -3086,11 +3086,11 @@
     <row r="14" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="28"/>
       <c r="B14" s="39" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C14" s="40"/>
       <c r="D14" s="41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="42">
         <v>43885</v>
@@ -3167,11 +3167,11 @@
     <row r="15" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="28"/>
       <c r="B15" s="39" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C15" s="40"/>
       <c r="D15" s="41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="42">
         <v>43885</v>
@@ -3999,7 +3999,7 @@
     <row r="25" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="28"/>
       <c r="B25" s="55" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C25" s="56"/>
       <c r="D25" s="57">
@@ -5162,8 +5162,8 @@
     </row>
     <row r="39" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="28"/>
-      <c r="B39" s="75" t="s">
-        <v>76</v>
+      <c r="B39" s="68" t="s">
+        <v>73</v>
       </c>
       <c r="C39" s="64"/>
       <c r="D39" s="65">
@@ -5327,7 +5327,7 @@
     <row r="41" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="28"/>
       <c r="B41" s="63" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C41" s="64"/>
       <c r="D41" s="65">
@@ -5411,7 +5411,7 @@
     <row r="42" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="28"/>
       <c r="B42" s="63" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C42" s="64"/>
       <c r="D42" s="65">
@@ -5494,8 +5494,8 @@
     </row>
     <row r="43" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="28"/>
-      <c r="B43" s="75" t="s">
-        <v>77</v>
+      <c r="B43" s="68" t="s">
+        <v>74</v>
       </c>
       <c r="C43" s="64"/>
       <c r="D43" s="65">
@@ -5656,7 +5656,7 @@
     </row>
     <row r="45" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B45" s="63" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C45" s="64"/>
       <c r="D45" s="65">
@@ -5739,7 +5739,7 @@
     </row>
     <row r="46" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B46" s="63" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C46" s="64"/>
       <c r="D46" s="65">
@@ -5822,7 +5822,7 @@
     </row>
     <row r="47" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B47" s="63" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C47" s="64"/>
       <c r="D47" s="65">
@@ -6065,6 +6065,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="BM4:BS4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
@@ -6073,11 +6078,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="D7">

</xml_diff>

<commit_message>
Completed skeleton implimentation for HomeAlarm, ready to function with other sensor/alarm classes. Added Status enum for HomeAlarm to use. Edited gant chart to reflect work. Deleted NRevisedCS401ProjectChart.xlsx because it was an old version of our running Gant Chart.
</commit_message>
<xml_diff>
--- a/CS401ProjectGnattChart.xlsx
+++ b/CS401ProjectGnattChart.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="154" documentId="13_ncr:1_{93D8DC03-8DEF-45F2-8570-FF4EF3D5A7AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{30FDB64F-CD98-4F5D-8587-BFAFE0986624}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E7AFE3-F7B1-3D41-8E4C-048151EAED78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -316,13 +316,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="ddd\,\ m/d/yyyy"/>
     <numFmt numFmtId="166" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="167" formatCode="d"/>
-    <numFmt numFmtId="168" formatCode="m/d/yy"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -829,7 +828,7 @@
     <xf numFmtId="9" fontId="22" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -841,7 +840,7 @@
     <xf numFmtId="9" fontId="22" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -853,7 +852,7 @@
     <xf numFmtId="9" fontId="22" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -865,7 +864,7 @@
     <xf numFmtId="9" fontId="22" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -877,7 +876,7 @@
     <xf numFmtId="9" fontId="22" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -889,7 +888,7 @@
     <xf numFmtId="9" fontId="22" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -901,7 +900,7 @@
     <xf numFmtId="9" fontId="22" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -913,7 +912,7 @@
     <xf numFmtId="9" fontId="22" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="22" fillId="6" borderId="11" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -922,6 +921,13 @@
     <xf numFmtId="0" fontId="23" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="7" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -934,13 +940,6 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="8" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="7" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="3" builtinId="3" customBuiltin="1"/>
@@ -1810,24 +1809,24 @@
   <dimension ref="A1:BS49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="83" zoomScaleNormal="40" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" style="28" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" customWidth="1"/>
-    <col min="3" max="3" width="30.7265625" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" customWidth="1"/>
-    <col min="7" max="7" width="2.7265625" customWidth="1"/>
-    <col min="8" max="8" width="6.1796875" hidden="1" customWidth="1"/>
-    <col min="9" max="71" width="2.54296875" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="71" width="2.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="29" t="s">
         <v>24</v>
       </c>
@@ -1843,7 +1842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>22</v>
       </c>
@@ -1854,132 +1853,132 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="34"/>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="74"/>
-      <c r="E3" s="72">
+      <c r="D3" s="70"/>
+      <c r="E3" s="75">
         <v>43878</v>
       </c>
-      <c r="F3" s="72"/>
+      <c r="F3" s="75"/>
     </row>
-    <row r="4" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="74"/>
+      <c r="D4" s="70"/>
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="69">
+      <c r="I4" s="72">
         <f>I5</f>
         <v>43878</v>
       </c>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
-      <c r="O4" s="71"/>
-      <c r="P4" s="69">
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="72">
         <f>P5</f>
         <v>43885</v>
       </c>
-      <c r="Q4" s="70"/>
-      <c r="R4" s="70"/>
-      <c r="S4" s="70"/>
-      <c r="T4" s="70"/>
-      <c r="U4" s="70"/>
-      <c r="V4" s="71"/>
-      <c r="W4" s="69">
+      <c r="Q4" s="73"/>
+      <c r="R4" s="73"/>
+      <c r="S4" s="73"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="73"/>
+      <c r="V4" s="74"/>
+      <c r="W4" s="72">
         <f>W5</f>
         <v>43892</v>
       </c>
-      <c r="X4" s="70"/>
-      <c r="Y4" s="70"/>
-      <c r="Z4" s="70"/>
-      <c r="AA4" s="70"/>
-      <c r="AB4" s="70"/>
-      <c r="AC4" s="71"/>
-      <c r="AD4" s="69">
+      <c r="X4" s="73"/>
+      <c r="Y4" s="73"/>
+      <c r="Z4" s="73"/>
+      <c r="AA4" s="73"/>
+      <c r="AB4" s="73"/>
+      <c r="AC4" s="74"/>
+      <c r="AD4" s="72">
         <f>AD5</f>
         <v>43899</v>
       </c>
-      <c r="AE4" s="70"/>
-      <c r="AF4" s="70"/>
-      <c r="AG4" s="70"/>
-      <c r="AH4" s="70"/>
-      <c r="AI4" s="70"/>
-      <c r="AJ4" s="71"/>
-      <c r="AK4" s="69">
+      <c r="AE4" s="73"/>
+      <c r="AF4" s="73"/>
+      <c r="AG4" s="73"/>
+      <c r="AH4" s="73"/>
+      <c r="AI4" s="73"/>
+      <c r="AJ4" s="74"/>
+      <c r="AK4" s="72">
         <f>AK5</f>
         <v>43906</v>
       </c>
-      <c r="AL4" s="70"/>
-      <c r="AM4" s="70"/>
-      <c r="AN4" s="70"/>
-      <c r="AO4" s="70"/>
-      <c r="AP4" s="70"/>
-      <c r="AQ4" s="71"/>
-      <c r="AR4" s="69">
+      <c r="AL4" s="73"/>
+      <c r="AM4" s="73"/>
+      <c r="AN4" s="73"/>
+      <c r="AO4" s="73"/>
+      <c r="AP4" s="73"/>
+      <c r="AQ4" s="74"/>
+      <c r="AR4" s="72">
         <f>AR5</f>
         <v>43913</v>
       </c>
-      <c r="AS4" s="70"/>
-      <c r="AT4" s="70"/>
-      <c r="AU4" s="70"/>
-      <c r="AV4" s="70"/>
-      <c r="AW4" s="70"/>
-      <c r="AX4" s="71"/>
-      <c r="AY4" s="69">
+      <c r="AS4" s="73"/>
+      <c r="AT4" s="73"/>
+      <c r="AU4" s="73"/>
+      <c r="AV4" s="73"/>
+      <c r="AW4" s="73"/>
+      <c r="AX4" s="74"/>
+      <c r="AY4" s="72">
         <f>AY5</f>
         <v>43920</v>
       </c>
-      <c r="AZ4" s="70"/>
-      <c r="BA4" s="70"/>
-      <c r="BB4" s="70"/>
-      <c r="BC4" s="70"/>
-      <c r="BD4" s="70"/>
-      <c r="BE4" s="71"/>
-      <c r="BF4" s="69">
+      <c r="AZ4" s="73"/>
+      <c r="BA4" s="73"/>
+      <c r="BB4" s="73"/>
+      <c r="BC4" s="73"/>
+      <c r="BD4" s="73"/>
+      <c r="BE4" s="74"/>
+      <c r="BF4" s="72">
         <f>BF5</f>
         <v>43927</v>
       </c>
-      <c r="BG4" s="70"/>
-      <c r="BH4" s="70"/>
-      <c r="BI4" s="70"/>
-      <c r="BJ4" s="70"/>
-      <c r="BK4" s="70"/>
-      <c r="BL4" s="71"/>
-      <c r="BM4" s="69">
+      <c r="BG4" s="73"/>
+      <c r="BH4" s="73"/>
+      <c r="BI4" s="73"/>
+      <c r="BJ4" s="73"/>
+      <c r="BK4" s="73"/>
+      <c r="BL4" s="74"/>
+      <c r="BM4" s="72">
         <f>BM5</f>
         <v>43934</v>
       </c>
-      <c r="BN4" s="70"/>
-      <c r="BO4" s="70"/>
-      <c r="BP4" s="70"/>
-      <c r="BQ4" s="70"/>
-      <c r="BR4" s="70"/>
-      <c r="BS4" s="71"/>
+      <c r="BN4" s="73"/>
+      <c r="BO4" s="73"/>
+      <c r="BP4" s="73"/>
+      <c r="BQ4" s="73"/>
+      <c r="BR4" s="73"/>
+      <c r="BS4" s="74"/>
     </row>
-    <row r="5" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
       <c r="I5" s="10">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43878</v>
@@ -2233,7 +2232,7 @@
         <v>43940</v>
       </c>
     </row>
-    <row r="6" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>28</v>
       </c>
@@ -2507,7 +2506,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:71" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:71" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>23</v>
       </c>
@@ -2581,7 +2580,7 @@
       <c r="BR7" s="15"/>
       <c r="BS7" s="15"/>
     </row>
-    <row r="8" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>29</v>
       </c>
@@ -2661,7 +2660,7 @@
       <c r="BR8" s="15"/>
       <c r="BS8" s="15"/>
     </row>
-    <row r="9" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>30</v>
       </c>
@@ -2748,7 +2747,7 @@
       <c r="BR9" s="15"/>
       <c r="BS9" s="15"/>
     </row>
-    <row r="10" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>31</v>
       </c>
@@ -2834,7 +2833,7 @@
       <c r="BR10" s="15"/>
       <c r="BS10" s="15"/>
     </row>
-    <row r="11" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="39" t="s">
         <v>38</v>
@@ -2918,7 +2917,7 @@
       <c r="BR11" s="15"/>
       <c r="BS11" s="15"/>
     </row>
-    <row r="12" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28"/>
       <c r="B12" s="39" t="s">
         <v>39</v>
@@ -3002,7 +3001,7 @@
       <c r="BR12" s="15"/>
       <c r="BS12" s="15"/>
     </row>
-    <row r="13" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28"/>
       <c r="B13" s="39" t="s">
         <v>75</v>
@@ -3083,7 +3082,7 @@
       <c r="BR13" s="15"/>
       <c r="BS13" s="15"/>
     </row>
-    <row r="14" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="28"/>
       <c r="B14" s="39" t="s">
         <v>76</v>
@@ -3164,7 +3163,7 @@
       <c r="BR14" s="15"/>
       <c r="BS14" s="15"/>
     </row>
-    <row r="15" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="39" t="s">
         <v>77</v>
@@ -3248,7 +3247,7 @@
       <c r="BR15" s="15"/>
       <c r="BS15" s="15"/>
     </row>
-    <row r="16" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>32</v>
       </c>
@@ -3328,7 +3327,7 @@
       <c r="BR16" s="15"/>
       <c r="BS16" s="15"/>
     </row>
-    <row r="17" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
       <c r="B17" s="47" t="s">
         <v>40</v>
@@ -3412,14 +3411,14 @@
       <c r="BR17" s="15"/>
       <c r="BS17" s="15"/>
     </row>
-    <row r="18" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="28"/>
       <c r="B18" s="47" t="s">
         <v>41</v>
       </c>
       <c r="C18" s="48"/>
       <c r="D18" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="50">
         <v>43892</v>
@@ -3496,7 +3495,7 @@
       <c r="BR18" s="15"/>
       <c r="BS18" s="15"/>
     </row>
-    <row r="19" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="28"/>
       <c r="B19" s="47" t="s">
         <v>42</v>
@@ -3580,7 +3579,7 @@
       <c r="BR19" s="15"/>
       <c r="BS19" s="15"/>
     </row>
-    <row r="20" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="28"/>
       <c r="B20" s="47" t="s">
         <v>58</v>
@@ -3664,7 +3663,7 @@
       <c r="BR20" s="15"/>
       <c r="BS20" s="15"/>
     </row>
-    <row r="21" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
         <v>44</v>
       </c>
@@ -3744,7 +3743,7 @@
       <c r="BR21" s="15"/>
       <c r="BS21" s="15"/>
     </row>
-    <row r="22" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="28"/>
       <c r="B22" s="55" t="s">
         <v>59</v>
@@ -3828,7 +3827,7 @@
       <c r="BR22" s="15"/>
       <c r="BS22" s="15"/>
     </row>
-    <row r="23" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
       <c r="B23" s="55" t="s">
         <v>46</v>
@@ -3912,7 +3911,7 @@
       <c r="BR23" s="15"/>
       <c r="BS23" s="15"/>
     </row>
-    <row r="24" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="28"/>
       <c r="B24" s="55" t="s">
         <v>47</v>
@@ -3996,7 +3995,7 @@
       <c r="BR24" s="15"/>
       <c r="BS24" s="15"/>
     </row>
-    <row r="25" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="28"/>
       <c r="B25" s="55" t="s">
         <v>72</v>
@@ -4080,7 +4079,7 @@
       <c r="BR25" s="15"/>
       <c r="BS25" s="15"/>
     </row>
-    <row r="26" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
         <v>48</v>
       </c>
@@ -4160,7 +4159,7 @@
       <c r="BR26" s="15"/>
       <c r="BS26" s="15"/>
     </row>
-    <row r="27" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="28"/>
       <c r="B27" s="63" t="s">
         <v>50</v>
@@ -4244,7 +4243,7 @@
       <c r="BR27" s="15"/>
       <c r="BS27" s="15"/>
     </row>
-    <row r="28" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="28"/>
       <c r="B28" s="63" t="s">
         <v>51</v>
@@ -4328,7 +4327,7 @@
       <c r="BR28" s="15"/>
       <c r="BS28" s="15"/>
     </row>
-    <row r="29" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28"/>
       <c r="B29" s="63" t="s">
         <v>60</v>
@@ -4412,7 +4411,7 @@
       <c r="BR29" s="15"/>
       <c r="BS29" s="15"/>
     </row>
-    <row r="30" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28"/>
       <c r="B30" s="63" t="s">
         <v>52</v>
@@ -4496,7 +4495,7 @@
       <c r="BR30" s="15"/>
       <c r="BS30" s="15"/>
     </row>
-    <row r="31" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="28"/>
       <c r="B31" s="63" t="s">
         <v>53</v>
@@ -4580,7 +4579,7 @@
       <c r="BR31" s="15"/>
       <c r="BS31" s="15"/>
     </row>
-    <row r="32" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>48</v>
       </c>
@@ -4660,7 +4659,7 @@
       <c r="BR32" s="15"/>
       <c r="BS32" s="15"/>
     </row>
-    <row r="33" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="28"/>
       <c r="B33" s="63" t="s">
         <v>61</v>
@@ -4744,7 +4743,7 @@
       <c r="BR33" s="15"/>
       <c r="BS33" s="15"/>
     </row>
-    <row r="34" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="28"/>
       <c r="B34" s="63" t="s">
         <v>62</v>
@@ -4828,7 +4827,7 @@
       <c r="BR34" s="15"/>
       <c r="BS34" s="15"/>
     </row>
-    <row r="35" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="28"/>
       <c r="B35" s="63" t="s">
         <v>63</v>
@@ -4912,7 +4911,7 @@
       <c r="BR35" s="15"/>
       <c r="BS35" s="15"/>
     </row>
-    <row r="36" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
         <v>48</v>
       </c>
@@ -4992,7 +4991,7 @@
       <c r="BR36" s="15"/>
       <c r="BS36" s="15"/>
     </row>
-    <row r="37" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="28"/>
       <c r="B37" s="63" t="s">
         <v>64</v>
@@ -5076,7 +5075,7 @@
       <c r="BR37" s="15"/>
       <c r="BS37" s="15"/>
     </row>
-    <row r="38" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="28"/>
       <c r="B38" s="63" t="s">
         <v>65</v>
@@ -5160,7 +5159,7 @@
       <c r="BR38" s="15"/>
       <c r="BS38" s="15"/>
     </row>
-    <row r="39" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
       <c r="B39" s="68" t="s">
         <v>73</v>
@@ -5244,7 +5243,7 @@
       <c r="BR39" s="15"/>
       <c r="BS39" s="15"/>
     </row>
-    <row r="40" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
         <v>48</v>
       </c>
@@ -5324,7 +5323,7 @@
       <c r="BR40" s="15"/>
       <c r="BS40" s="15"/>
     </row>
-    <row r="41" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="28"/>
       <c r="B41" s="63" t="s">
         <v>71</v>
@@ -5408,7 +5407,7 @@
       <c r="BR41" s="15"/>
       <c r="BS41" s="15"/>
     </row>
-    <row r="42" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="28"/>
       <c r="B42" s="63" t="s">
         <v>70</v>
@@ -5492,7 +5491,7 @@
       <c r="BR42" s="15"/>
       <c r="BS42" s="15"/>
     </row>
-    <row r="43" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="28"/>
       <c r="B43" s="68" t="s">
         <v>74</v>
@@ -5576,7 +5575,7 @@
       <c r="BR43" s="15"/>
       <c r="BS43" s="15"/>
     </row>
-    <row r="44" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="28"/>
       <c r="B44" s="59" t="s">
         <v>56</v>
@@ -5654,7 +5653,7 @@
       <c r="BR44" s="15"/>
       <c r="BS44" s="15"/>
     </row>
-    <row r="45" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="63" t="s">
         <v>67</v>
       </c>
@@ -5737,7 +5736,7 @@
       <c r="BR45" s="15"/>
       <c r="BS45" s="15"/>
     </row>
-    <row r="46" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="63" t="s">
         <v>68</v>
       </c>
@@ -5820,7 +5819,7 @@
       <c r="BR46" s="15"/>
       <c r="BS46" s="15"/>
     </row>
-    <row r="47" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="63" t="s">
         <v>69</v>
       </c>
@@ -5903,7 +5902,7 @@
       <c r="BR47" s="15"/>
       <c r="BS47" s="15"/>
     </row>
-    <row r="48" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="59" t="s">
         <v>57</v>
       </c>
@@ -5980,7 +5979,7 @@
       <c r="BR48" s="15"/>
       <c r="BS48" s="15"/>
     </row>
-    <row r="49" spans="2:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="63" t="s">
         <v>66</v>
       </c>
@@ -6065,11 +6064,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="BM4:BS4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
@@ -6078,6 +6072,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="D7">
@@ -6282,86 +6281,86 @@
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="87.1796875" style="18" customWidth="1"/>
-    <col min="2" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="87.1640625" style="18" customWidth="1"/>
+    <col min="2" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:2" s="20" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:2" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="19"/>
     </row>
-    <row r="3" spans="1:2" s="24" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" s="24" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="25"/>
     </row>
-    <row r="4" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="18" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" s="18" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="58" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="72.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Edited Gant Chart to reflect everyone has completed their task for the week of March 8
</commit_message>
<xml_diff>
--- a/CS401ProjectGnattChart.xlsx
+++ b/CS401ProjectGnattChart.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{93D8DC03-8DEF-45F2-8570-FF4EF3D5A7AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6534FE33-BB72-4262-9139-813AB69308DB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F0732A-39B7-1545-A79B-28323DF39E1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7720" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -316,13 +316,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="ddd\,\ m/d/yyyy"/>
     <numFmt numFmtId="166" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="167" formatCode="d"/>
-    <numFmt numFmtId="168" formatCode="m/d/yy"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -829,7 +828,7 @@
     <xf numFmtId="9" fontId="22" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -841,7 +840,7 @@
     <xf numFmtId="9" fontId="22" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -853,7 +852,7 @@
     <xf numFmtId="9" fontId="22" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -865,7 +864,7 @@
     <xf numFmtId="9" fontId="22" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -877,7 +876,7 @@
     <xf numFmtId="9" fontId="22" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -889,7 +888,7 @@
     <xf numFmtId="9" fontId="22" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -901,7 +900,7 @@
     <xf numFmtId="9" fontId="22" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -913,7 +912,7 @@
     <xf numFmtId="9" fontId="22" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="22" fillId="6" borderId="11" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -922,6 +921,18 @@
     <xf numFmtId="0" fontId="23" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="8" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -929,18 +940,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="8" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="3" builtinId="3" customBuiltin="1"/>
@@ -1810,24 +1809,24 @@
   <dimension ref="A1:BS49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="83" zoomScaleNormal="40" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" style="28" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" customWidth="1"/>
-    <col min="3" max="3" width="30.7265625" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" customWidth="1"/>
-    <col min="7" max="7" width="2.7265625" customWidth="1"/>
-    <col min="8" max="8" width="6.1796875" hidden="1" customWidth="1"/>
-    <col min="9" max="71" width="2.54296875" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="71" width="2.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="29" t="s">
         <v>24</v>
       </c>
@@ -1843,7 +1842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>22</v>
       </c>
@@ -1854,132 +1853,132 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="34"/>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="70"/>
-      <c r="E3" s="75">
+      <c r="D3" s="74"/>
+      <c r="E3" s="72">
         <v>43878</v>
       </c>
-      <c r="F3" s="75"/>
+      <c r="F3" s="72"/>
     </row>
-    <row r="4" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="70"/>
+      <c r="D4" s="74"/>
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="72">
+      <c r="I4" s="69">
         <f>I5</f>
         <v>43878</v>
       </c>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="72">
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="70"/>
+      <c r="O4" s="71"/>
+      <c r="P4" s="69">
         <f>P5</f>
         <v>43885</v>
       </c>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="73"/>
-      <c r="V4" s="74"/>
-      <c r="W4" s="72">
+      <c r="Q4" s="70"/>
+      <c r="R4" s="70"/>
+      <c r="S4" s="70"/>
+      <c r="T4" s="70"/>
+      <c r="U4" s="70"/>
+      <c r="V4" s="71"/>
+      <c r="W4" s="69">
         <f>W5</f>
         <v>43892</v>
       </c>
-      <c r="X4" s="73"/>
-      <c r="Y4" s="73"/>
-      <c r="Z4" s="73"/>
-      <c r="AA4" s="73"/>
-      <c r="AB4" s="73"/>
-      <c r="AC4" s="74"/>
-      <c r="AD4" s="72">
+      <c r="X4" s="70"/>
+      <c r="Y4" s="70"/>
+      <c r="Z4" s="70"/>
+      <c r="AA4" s="70"/>
+      <c r="AB4" s="70"/>
+      <c r="AC4" s="71"/>
+      <c r="AD4" s="69">
         <f>AD5</f>
         <v>43899</v>
       </c>
-      <c r="AE4" s="73"/>
-      <c r="AF4" s="73"/>
-      <c r="AG4" s="73"/>
-      <c r="AH4" s="73"/>
-      <c r="AI4" s="73"/>
-      <c r="AJ4" s="74"/>
-      <c r="AK4" s="72">
+      <c r="AE4" s="70"/>
+      <c r="AF4" s="70"/>
+      <c r="AG4" s="70"/>
+      <c r="AH4" s="70"/>
+      <c r="AI4" s="70"/>
+      <c r="AJ4" s="71"/>
+      <c r="AK4" s="69">
         <f>AK5</f>
         <v>43906</v>
       </c>
-      <c r="AL4" s="73"/>
-      <c r="AM4" s="73"/>
-      <c r="AN4" s="73"/>
-      <c r="AO4" s="73"/>
-      <c r="AP4" s="73"/>
-      <c r="AQ4" s="74"/>
-      <c r="AR4" s="72">
+      <c r="AL4" s="70"/>
+      <c r="AM4" s="70"/>
+      <c r="AN4" s="70"/>
+      <c r="AO4" s="70"/>
+      <c r="AP4" s="70"/>
+      <c r="AQ4" s="71"/>
+      <c r="AR4" s="69">
         <f>AR5</f>
         <v>43913</v>
       </c>
-      <c r="AS4" s="73"/>
-      <c r="AT4" s="73"/>
-      <c r="AU4" s="73"/>
-      <c r="AV4" s="73"/>
-      <c r="AW4" s="73"/>
-      <c r="AX4" s="74"/>
-      <c r="AY4" s="72">
+      <c r="AS4" s="70"/>
+      <c r="AT4" s="70"/>
+      <c r="AU4" s="70"/>
+      <c r="AV4" s="70"/>
+      <c r="AW4" s="70"/>
+      <c r="AX4" s="71"/>
+      <c r="AY4" s="69">
         <f>AY5</f>
         <v>43920</v>
       </c>
-      <c r="AZ4" s="73"/>
-      <c r="BA4" s="73"/>
-      <c r="BB4" s="73"/>
-      <c r="BC4" s="73"/>
-      <c r="BD4" s="73"/>
-      <c r="BE4" s="74"/>
-      <c r="BF4" s="72">
+      <c r="AZ4" s="70"/>
+      <c r="BA4" s="70"/>
+      <c r="BB4" s="70"/>
+      <c r="BC4" s="70"/>
+      <c r="BD4" s="70"/>
+      <c r="BE4" s="71"/>
+      <c r="BF4" s="69">
         <f>BF5</f>
         <v>43927</v>
       </c>
-      <c r="BG4" s="73"/>
-      <c r="BH4" s="73"/>
-      <c r="BI4" s="73"/>
-      <c r="BJ4" s="73"/>
-      <c r="BK4" s="73"/>
-      <c r="BL4" s="74"/>
-      <c r="BM4" s="72">
+      <c r="BG4" s="70"/>
+      <c r="BH4" s="70"/>
+      <c r="BI4" s="70"/>
+      <c r="BJ4" s="70"/>
+      <c r="BK4" s="70"/>
+      <c r="BL4" s="71"/>
+      <c r="BM4" s="69">
         <f>BM5</f>
         <v>43934</v>
       </c>
-      <c r="BN4" s="73"/>
-      <c r="BO4" s="73"/>
-      <c r="BP4" s="73"/>
-      <c r="BQ4" s="73"/>
-      <c r="BR4" s="73"/>
-      <c r="BS4" s="74"/>
+      <c r="BN4" s="70"/>
+      <c r="BO4" s="70"/>
+      <c r="BP4" s="70"/>
+      <c r="BQ4" s="70"/>
+      <c r="BR4" s="70"/>
+      <c r="BS4" s="71"/>
     </row>
-    <row r="5" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
       <c r="I5" s="10">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43878</v>
@@ -2233,7 +2232,7 @@
         <v>43940</v>
       </c>
     </row>
-    <row r="6" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>28</v>
       </c>
@@ -2507,7 +2506,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:71" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:71" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>23</v>
       </c>
@@ -2581,7 +2580,7 @@
       <c r="BR7" s="15"/>
       <c r="BS7" s="15"/>
     </row>
-    <row r="8" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>29</v>
       </c>
@@ -2661,7 +2660,7 @@
       <c r="BR8" s="15"/>
       <c r="BS8" s="15"/>
     </row>
-    <row r="9" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>30</v>
       </c>
@@ -2748,7 +2747,7 @@
       <c r="BR9" s="15"/>
       <c r="BS9" s="15"/>
     </row>
-    <row r="10" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>31</v>
       </c>
@@ -2834,7 +2833,7 @@
       <c r="BR10" s="15"/>
       <c r="BS10" s="15"/>
     </row>
-    <row r="11" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="39" t="s">
         <v>38</v>
@@ -2918,7 +2917,7 @@
       <c r="BR11" s="15"/>
       <c r="BS11" s="15"/>
     </row>
-    <row r="12" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28"/>
       <c r="B12" s="39" t="s">
         <v>39</v>
@@ -3002,7 +3001,7 @@
       <c r="BR12" s="15"/>
       <c r="BS12" s="15"/>
     </row>
-    <row r="13" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28"/>
       <c r="B13" s="39" t="s">
         <v>75</v>
@@ -3083,7 +3082,7 @@
       <c r="BR13" s="15"/>
       <c r="BS13" s="15"/>
     </row>
-    <row r="14" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="28"/>
       <c r="B14" s="39" t="s">
         <v>76</v>
@@ -3164,7 +3163,7 @@
       <c r="BR14" s="15"/>
       <c r="BS14" s="15"/>
     </row>
-    <row r="15" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="39" t="s">
         <v>77</v>
@@ -3248,7 +3247,7 @@
       <c r="BR15" s="15"/>
       <c r="BS15" s="15"/>
     </row>
-    <row r="16" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>32</v>
       </c>
@@ -3328,7 +3327,7 @@
       <c r="BR16" s="15"/>
       <c r="BS16" s="15"/>
     </row>
-    <row r="17" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
       <c r="B17" s="47" t="s">
         <v>40</v>
@@ -3412,14 +3411,14 @@
       <c r="BR17" s="15"/>
       <c r="BS17" s="15"/>
     </row>
-    <row r="18" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="28"/>
       <c r="B18" s="47" t="s">
         <v>41</v>
       </c>
       <c r="C18" s="48"/>
       <c r="D18" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="50">
         <v>43892</v>
@@ -3496,14 +3495,14 @@
       <c r="BR18" s="15"/>
       <c r="BS18" s="15"/>
     </row>
-    <row r="19" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="28"/>
       <c r="B19" s="47" t="s">
         <v>42</v>
       </c>
       <c r="C19" s="48"/>
       <c r="D19" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="50">
         <v>43892</v>
@@ -3580,7 +3579,7 @@
       <c r="BR19" s="15"/>
       <c r="BS19" s="15"/>
     </row>
-    <row r="20" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="28"/>
       <c r="B20" s="47" t="s">
         <v>58</v>
@@ -3664,7 +3663,7 @@
       <c r="BR20" s="15"/>
       <c r="BS20" s="15"/>
     </row>
-    <row r="21" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
         <v>44</v>
       </c>
@@ -3744,7 +3743,7 @@
       <c r="BR21" s="15"/>
       <c r="BS21" s="15"/>
     </row>
-    <row r="22" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="28"/>
       <c r="B22" s="55" t="s">
         <v>59</v>
@@ -3828,7 +3827,7 @@
       <c r="BR22" s="15"/>
       <c r="BS22" s="15"/>
     </row>
-    <row r="23" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
       <c r="B23" s="55" t="s">
         <v>46</v>
@@ -3912,7 +3911,7 @@
       <c r="BR23" s="15"/>
       <c r="BS23" s="15"/>
     </row>
-    <row r="24" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="28"/>
       <c r="B24" s="55" t="s">
         <v>47</v>
@@ -3996,7 +3995,7 @@
       <c r="BR24" s="15"/>
       <c r="BS24" s="15"/>
     </row>
-    <row r="25" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="28"/>
       <c r="B25" s="55" t="s">
         <v>72</v>
@@ -4080,7 +4079,7 @@
       <c r="BR25" s="15"/>
       <c r="BS25" s="15"/>
     </row>
-    <row r="26" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
         <v>48</v>
       </c>
@@ -4160,7 +4159,7 @@
       <c r="BR26" s="15"/>
       <c r="BS26" s="15"/>
     </row>
-    <row r="27" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="28"/>
       <c r="B27" s="63" t="s">
         <v>50</v>
@@ -4244,7 +4243,7 @@
       <c r="BR27" s="15"/>
       <c r="BS27" s="15"/>
     </row>
-    <row r="28" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="28"/>
       <c r="B28" s="63" t="s">
         <v>51</v>
@@ -4328,7 +4327,7 @@
       <c r="BR28" s="15"/>
       <c r="BS28" s="15"/>
     </row>
-    <row r="29" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28"/>
       <c r="B29" s="63" t="s">
         <v>60</v>
@@ -4412,7 +4411,7 @@
       <c r="BR29" s="15"/>
       <c r="BS29" s="15"/>
     </row>
-    <row r="30" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28"/>
       <c r="B30" s="63" t="s">
         <v>52</v>
@@ -4496,7 +4495,7 @@
       <c r="BR30" s="15"/>
       <c r="BS30" s="15"/>
     </row>
-    <row r="31" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="28"/>
       <c r="B31" s="63" t="s">
         <v>53</v>
@@ -4580,7 +4579,7 @@
       <c r="BR31" s="15"/>
       <c r="BS31" s="15"/>
     </row>
-    <row r="32" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>48</v>
       </c>
@@ -4660,7 +4659,7 @@
       <c r="BR32" s="15"/>
       <c r="BS32" s="15"/>
     </row>
-    <row r="33" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="28"/>
       <c r="B33" s="63" t="s">
         <v>61</v>
@@ -4744,7 +4743,7 @@
       <c r="BR33" s="15"/>
       <c r="BS33" s="15"/>
     </row>
-    <row r="34" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="28"/>
       <c r="B34" s="63" t="s">
         <v>62</v>
@@ -4828,7 +4827,7 @@
       <c r="BR34" s="15"/>
       <c r="BS34" s="15"/>
     </row>
-    <row r="35" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="28"/>
       <c r="B35" s="63" t="s">
         <v>63</v>
@@ -4912,7 +4911,7 @@
       <c r="BR35" s="15"/>
       <c r="BS35" s="15"/>
     </row>
-    <row r="36" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
         <v>48</v>
       </c>
@@ -4992,7 +4991,7 @@
       <c r="BR36" s="15"/>
       <c r="BS36" s="15"/>
     </row>
-    <row r="37" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="28"/>
       <c r="B37" s="63" t="s">
         <v>64</v>
@@ -5076,7 +5075,7 @@
       <c r="BR37" s="15"/>
       <c r="BS37" s="15"/>
     </row>
-    <row r="38" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="28"/>
       <c r="B38" s="63" t="s">
         <v>65</v>
@@ -5160,7 +5159,7 @@
       <c r="BR38" s="15"/>
       <c r="BS38" s="15"/>
     </row>
-    <row r="39" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
       <c r="B39" s="68" t="s">
         <v>73</v>
@@ -5244,7 +5243,7 @@
       <c r="BR39" s="15"/>
       <c r="BS39" s="15"/>
     </row>
-    <row r="40" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
         <v>48</v>
       </c>
@@ -5324,7 +5323,7 @@
       <c r="BR40" s="15"/>
       <c r="BS40" s="15"/>
     </row>
-    <row r="41" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="28"/>
       <c r="B41" s="63" t="s">
         <v>71</v>
@@ -5408,7 +5407,7 @@
       <c r="BR41" s="15"/>
       <c r="BS41" s="15"/>
     </row>
-    <row r="42" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="28"/>
       <c r="B42" s="63" t="s">
         <v>70</v>
@@ -5492,7 +5491,7 @@
       <c r="BR42" s="15"/>
       <c r="BS42" s="15"/>
     </row>
-    <row r="43" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="28"/>
       <c r="B43" s="68" t="s">
         <v>74</v>
@@ -5576,7 +5575,7 @@
       <c r="BR43" s="15"/>
       <c r="BS43" s="15"/>
     </row>
-    <row r="44" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="28"/>
       <c r="B44" s="59" t="s">
         <v>56</v>
@@ -5654,7 +5653,7 @@
       <c r="BR44" s="15"/>
       <c r="BS44" s="15"/>
     </row>
-    <row r="45" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="63" t="s">
         <v>67</v>
       </c>
@@ -5737,7 +5736,7 @@
       <c r="BR45" s="15"/>
       <c r="BS45" s="15"/>
     </row>
-    <row r="46" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="63" t="s">
         <v>68</v>
       </c>
@@ -5820,7 +5819,7 @@
       <c r="BR46" s="15"/>
       <c r="BS46" s="15"/>
     </row>
-    <row r="47" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="63" t="s">
         <v>69</v>
       </c>
@@ -5903,7 +5902,7 @@
       <c r="BR47" s="15"/>
       <c r="BS47" s="15"/>
     </row>
-    <row r="48" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="59" t="s">
         <v>57</v>
       </c>
@@ -5980,7 +5979,7 @@
       <c r="BR48" s="15"/>
       <c r="BS48" s="15"/>
     </row>
-    <row r="49" spans="2:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="63" t="s">
         <v>66</v>
       </c>
@@ -6065,6 +6064,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="BM4:BS4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
@@ -6073,11 +6077,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="D7">
@@ -6282,86 +6281,86 @@
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="87.1796875" style="18" customWidth="1"/>
-    <col min="2" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="87.1640625" style="18" customWidth="1"/>
+    <col min="2" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:2" s="20" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:2" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="19"/>
     </row>
-    <row r="3" spans="1:2" s="24" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" s="24" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="25"/>
     </row>
-    <row r="4" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="18" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" s="18" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="58" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="72.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>14</v>
       </c>

</xml_diff>